<commit_message>
Benchmarks für 60mio Datensatz ergänzt
</commit_message>
<xml_diff>
--- a/Laufzeit Benchmarks.xlsx
+++ b/Laufzeit Benchmarks.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,17 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7770" xr2:uid="{CF6F9929-A31F-489D-9572-F5B799929CF5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7770" activeTab="4" xr2:uid="{CF6F9929-A31F-489D-9572-F5B799929CF5}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
     <sheet name="Tabelle4" sheetId="4" r:id="rId4"/>
+    <sheet name="Tabelle5" sheetId="5" r:id="rId5"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId5"/>
-  </externalReferences>
   <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -30,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="47">
   <si>
     <t>Mit Daten kopieren</t>
   </si>
@@ -162,6 +160,15 @@
   </si>
   <si>
     <t xml:space="preserve"> CPU 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CPU</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> GPU</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> GPU mit kopieren</t>
   </si>
 </sst>
 </file>
@@ -347,15 +354,6 @@
     <xf numFmtId="2" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -366,6 +364,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -737,7 +744,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -791,7 +797,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="de-DE"/>
-                  <a:t>Partikel Anzahl</a:t>
+                  <a:t>Partikelanzahl</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1698,7 +1704,7 @@
                 <c:order val="3"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Tabelle2!$F$14</c15:sqref>
@@ -1763,7 +1769,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -1785,7 +1791,7 @@
                 </c:dLbls>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Tabelle2!$A$15:$A$24</c15:sqref>
@@ -1830,7 +1836,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Tabelle2!$F$15:$F$24</c15:sqref>
@@ -1874,7 +1880,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-608A-43E6-B652-0A8BC0A750C6}"/>
                   </c:ext>
@@ -1912,7 +1918,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="de-DE"/>
-                  <a:t>Partikel Anzahl</a:t>
+                  <a:t>Partikelanzahl</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2434,6 +2440,44 @@
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Hashgrid</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="de-DE" baseline="0"/>
+                  <a:t> Dimension</a:t>
+                </a:r>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.4453225439127802"/>
+              <c:y val="0.90547660004037955"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5417,7 +5461,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="de-DE"/>
-                  <a:t>Partikel Anzahl</a:t>
+                  <a:t>Partikelanzahl</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -5725,6 +5769,1236 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle5!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v> CPU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:cat>
+            <c:numRef>
+              <c:f>Tabelle5!$A$2:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>60</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle5!$B$2:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>284</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>357</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>423</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>501</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>566</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>643</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>686</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>742</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>812</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>891</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>964</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1003</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1061</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1134</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1212</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1287</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1365</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1411</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-00AE-40F3-B90E-AC15B4E29F11}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle5!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v> GPU mit kopieren</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.6198449612403101E-2"/>
+                  <c:y val="-3.2025880485869497E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000012-00AE-40F3-B90E-AC15B4E29F11}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.6198449612403101E-2"/>
+                  <c:y val="-3.202588048586965E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000010-00AE-40F3-B90E-AC15B4E29F11}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:cat>
+            <c:numRef>
+              <c:f>Tabelle5!$A$2:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>60</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle5!$C$2:$C$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>139</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>161</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>181</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>226</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>248</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>271</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>294</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>315</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>339</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>358</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>381</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>402</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>426</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>449</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-00AE-40F3-B90E-AC15B4E29F11}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle5!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v> GPU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.6198449612403101E-2"/>
+                  <c:y val="-2.37571466357403E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000011-00AE-40F3-B90E-AC15B4E29F11}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.6198449612403101E-2"/>
+                  <c:y val="-1.3421229323078801E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000013-00AE-40F3-B90E-AC15B4E29F11}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.6198449612403101E-2"/>
+                  <c:y val="-1.9622779710675851E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000014-00AE-40F3-B90E-AC15B4E29F11}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:cat>
+            <c:numRef>
+              <c:f>Tabelle5!$A$2:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>60</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle5!$D$2:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>153</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-00AE-40F3-B90E-AC15B4E29F11}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="543509480"/>
+        <c:axId val="543500952"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="543509480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Partikelanzahl in Millionen</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="543500952"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="543500952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1600"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Laufzeit in ms</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="543509480"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:minorUnit val="50"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -5885,6 +7159,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -7917,6 +9231,522 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -8100,128 +9930,45 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Tabelle1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="5">
-          <cell r="A5">
-            <v>2000000</v>
-          </cell>
-          <cell r="B5">
-            <v>20.64</v>
-          </cell>
-          <cell r="C5">
-            <v>123.917</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6">
-            <v>1800000</v>
-          </cell>
-          <cell r="B6">
-            <v>18.731999999999999</v>
-          </cell>
-          <cell r="C6">
-            <v>114.949</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7">
-            <v>1600000</v>
-          </cell>
-          <cell r="B7">
-            <v>16.920999999999999</v>
-          </cell>
-          <cell r="C7">
-            <v>103.092</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8">
-            <v>1400000</v>
-          </cell>
-          <cell r="B8">
-            <v>15.063000000000001</v>
-          </cell>
-          <cell r="C8">
-            <v>94.078000000000003</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9">
-            <v>1200000</v>
-          </cell>
-          <cell r="B9">
-            <v>13.119</v>
-          </cell>
-          <cell r="C9">
-            <v>85.269000000000005</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10">
-            <v>1000000</v>
-          </cell>
-          <cell r="B10">
-            <v>11.324</v>
-          </cell>
-          <cell r="C10">
-            <v>76.700999999999993</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11">
-            <v>800000</v>
-          </cell>
-          <cell r="B11">
-            <v>9.5</v>
-          </cell>
-          <cell r="C11">
-            <v>66.156999999999996</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12">
-            <v>600000</v>
-          </cell>
-          <cell r="B12">
-            <v>7.62</v>
-          </cell>
-          <cell r="C12">
-            <v>56.189</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="A13">
-            <v>400000</v>
-          </cell>
-          <cell r="B13">
-            <v>5.6079999999999997</v>
-          </cell>
-          <cell r="C13">
-            <v>43.987000000000002</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="A14">
-            <v>200000</v>
-          </cell>
-          <cell r="B14">
-            <v>3.84</v>
-          </cell>
-          <cell r="C14">
-            <v>27.097999999999999</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>314324</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>647699</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Diagramm 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6272BB7C-5DA6-4559-8BD5-9F288248D974}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8523,49 +10270,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DDBFD6F-1AC2-4396-A59E-40555DBC7422}">
   <dimension ref="A1:R22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
     </row>
     <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="47"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="51"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="48">
+      <c r="B4" s="45">
         <v>20</v>
       </c>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="49"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="46"/>
       <c r="H4" s="19" t="s">
         <v>0</v>
       </c>
@@ -8588,12 +10335,12 @@
       <c r="A5" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="49"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="46"/>
       <c r="H5" s="22" t="s">
         <v>2</v>
       </c>
@@ -8628,12 +10375,12 @@
       <c r="A6" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="49"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="46"/>
       <c r="H6" s="25">
         <v>200000</v>
       </c>
@@ -8671,12 +10418,12 @@
       <c r="A7" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="48" t="s">
+      <c r="B7" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="48"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="49"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="46"/>
       <c r="H7" s="25">
         <v>400000</v>
       </c>
@@ -8714,12 +10461,12 @@
       <c r="A8" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="48" t="s">
+      <c r="B8" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="48"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="49"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="46"/>
       <c r="H8" s="25">
         <v>600000</v>
       </c>
@@ -8757,12 +10504,12 @@
       <c r="A9" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="50" t="s">
+      <c r="B9" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="51"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="48"/>
       <c r="H9" s="25">
         <v>800000</v>
       </c>
@@ -9031,23 +10778,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="49"/>
+      <c r="O1" s="49"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -9059,78 +10806,78 @@
       <c r="A4" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="47"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="51"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="48">
+      <c r="B5" s="45">
         <v>20</v>
       </c>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="49"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="46"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="49"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="46"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="48" t="s">
+      <c r="B7" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="48"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="49"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="46"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="48" t="s">
+      <c r="B8" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="48"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="49"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="46"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="48" t="s">
+      <c r="B9" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="48"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="49"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="46"/>
     </row>
     <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="50" t="s">
+      <c r="B10" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="50"/>
-      <c r="D10" s="50"/>
-      <c r="E10" s="51"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="48"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
@@ -9163,7 +10910,7 @@
         <v>3.8460000000000001</v>
       </c>
       <c r="D15">
-        <f>ABS(C15-B15)</f>
+        <f t="shared" ref="D15:D24" si="0">ABS(C15-B15)</f>
         <v>6.0000000000002274E-3</v>
       </c>
       <c r="E15" s="2">
@@ -9173,7 +10920,7 @@
         <v>26.454000000000001</v>
       </c>
       <c r="G15">
-        <f>ABS(F15-E15)</f>
+        <f t="shared" ref="G15:G24" si="1">ABS(F15-E15)</f>
         <v>0.64399999999999835</v>
       </c>
     </row>
@@ -9188,7 +10935,7 @@
         <v>5.7610000000000001</v>
       </c>
       <c r="D16">
-        <f>ABS(C16-B16)</f>
+        <f t="shared" si="0"/>
         <v>0.15300000000000047</v>
       </c>
       <c r="E16" s="2">
@@ -9198,7 +10945,7 @@
         <v>43.322000000000003</v>
       </c>
       <c r="G16">
-        <f>ABS(F16-E16)</f>
+        <f t="shared" si="1"/>
         <v>0.66499999999999915</v>
       </c>
     </row>
@@ -9213,7 +10960,7 @@
         <v>7.5789999999999997</v>
       </c>
       <c r="D17">
-        <f>ABS(C17-B17)</f>
+        <f t="shared" si="0"/>
         <v>4.1000000000000369E-2</v>
       </c>
       <c r="E17" s="2">
@@ -9223,7 +10970,7 @@
         <v>55.795000000000002</v>
       </c>
       <c r="G17">
-        <f>ABS(F17-E17)</f>
+        <f t="shared" si="1"/>
         <v>0.39399999999999835</v>
       </c>
     </row>
@@ -9238,7 +10985,7 @@
         <v>9.3320000000000007</v>
       </c>
       <c r="D18">
-        <f>ABS(C18-B18)</f>
+        <f t="shared" si="0"/>
         <v>0.16799999999999926</v>
       </c>
       <c r="E18" s="2">
@@ -9248,7 +10995,7 @@
         <v>66.209000000000003</v>
       </c>
       <c r="G18">
-        <f>ABS(F18-E18)</f>
+        <f t="shared" si="1"/>
         <v>5.2000000000006708E-2</v>
       </c>
     </row>
@@ -9263,7 +11010,7 @@
         <v>11.244</v>
       </c>
       <c r="D19">
-        <f>ABS(C19-B19)</f>
+        <f t="shared" si="0"/>
         <v>8.0000000000000071E-2</v>
       </c>
       <c r="E19" s="2">
@@ -9273,7 +11020,7 @@
         <v>76.269000000000005</v>
       </c>
       <c r="G19">
-        <f>ABS(F19-E19)</f>
+        <f t="shared" si="1"/>
         <v>0.43199999999998795</v>
       </c>
     </row>
@@ -9288,7 +11035,7 @@
         <v>13.282</v>
       </c>
       <c r="D20">
-        <f>ABS(C20-B20)</f>
+        <f t="shared" si="0"/>
         <v>0.16300000000000026</v>
       </c>
       <c r="E20" s="2">
@@ -9298,7 +11045,7 @@
         <v>86.52</v>
       </c>
       <c r="G20">
-        <f>ABS(F20-E20)</f>
+        <f t="shared" si="1"/>
         <v>1.2509999999999906</v>
       </c>
     </row>
@@ -9313,7 +11060,7 @@
         <v>15.153</v>
       </c>
       <c r="D21">
-        <f>ABS(C21-B21)</f>
+        <f t="shared" si="0"/>
         <v>8.9999999999999858E-2</v>
       </c>
       <c r="E21" s="2">
@@ -9323,7 +11070,7 @@
         <v>92.811000000000007</v>
       </c>
       <c r="G21">
-        <f>ABS(F21-E21)</f>
+        <f t="shared" si="1"/>
         <v>1.2669999999999959</v>
       </c>
     </row>
@@ -9338,7 +11085,7 @@
         <v>16.954000000000001</v>
       </c>
       <c r="D22">
-        <f>ABS(C22-B22)</f>
+        <f t="shared" si="0"/>
         <v>3.3000000000001251E-2</v>
       </c>
       <c r="E22" s="2">
@@ -9348,7 +11095,7 @@
         <v>103.947</v>
       </c>
       <c r="G22">
-        <f>ABS(F22-E22)</f>
+        <f t="shared" si="1"/>
         <v>0.85500000000000398</v>
       </c>
     </row>
@@ -9363,7 +11110,7 @@
         <v>18.489000000000001</v>
       </c>
       <c r="D23">
-        <f>ABS(C23-B23)</f>
+        <f t="shared" si="0"/>
         <v>0.24299999999999855</v>
       </c>
       <c r="E23" s="2">
@@ -9373,7 +11120,7 @@
         <v>114.711</v>
       </c>
       <c r="G23">
-        <f>ABS(F23-E23)</f>
+        <f t="shared" si="1"/>
         <v>0.23799999999999955</v>
       </c>
     </row>
@@ -9388,7 +11135,7 @@
         <v>20.282</v>
       </c>
       <c r="D24">
-        <f>ABS(C24-B24)</f>
+        <f t="shared" si="0"/>
         <v>0.35800000000000054</v>
       </c>
       <c r="E24" s="2">
@@ -9398,7 +11145,7 @@
         <v>125.229</v>
       </c>
       <c r="G24">
-        <f>ABS(F24-E24)</f>
+        <f t="shared" si="1"/>
         <v>1.3119999999999976</v>
       </c>
     </row>
@@ -9435,101 +11182,101 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="49"/>
+      <c r="O1" s="49"/>
     </row>
     <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="47"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="51"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="48">
+      <c r="B4" s="45">
         <v>20</v>
       </c>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="49"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="46"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="48">
+      <c r="B5" s="45">
         <v>2000000</v>
       </c>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="49"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="46"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="49"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="46"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="48" t="s">
+      <c r="B7" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="48"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="49"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="46"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="48" t="s">
+      <c r="B8" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="48"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="49"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="46"/>
     </row>
     <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="50" t="s">
+      <c r="B9" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="51"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="48"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
@@ -9697,78 +11444,78 @@
       <c r="A3" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="47"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="51"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="48">
+      <c r="B4" s="45">
         <v>20</v>
       </c>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="49"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="46"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="49"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="46"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="49"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="46"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="48" t="s">
+      <c r="B7" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="48"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="49"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="46"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="48" t="s">
+      <c r="B8" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="48"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="49"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="46"/>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="50" t="s">
+      <c r="B9" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="51"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="48"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -11486,4 +13233,677 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B451884F-F8BD-4F01-B10F-A7E0BAE46247}">
+  <dimension ref="A1:D42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <f>A23/1000000</f>
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <f t="shared" ref="B2:D21" si="0">ROUND(B23/1000, 0)</f>
+        <v>128</v>
+      </c>
+      <c r="C2">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="D2">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f t="shared" ref="A3:A21" si="1">A24/1000000</f>
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <f t="shared" si="0"/>
+        <v>210</v>
+      </c>
+      <c r="C3">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="D3">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>284</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>357</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>93</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>423</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>117</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>501</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>139</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>566</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>161</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>643</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>181</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>686</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>205</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>742</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>226</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>812</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>248</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>891</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>271</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>964</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>294</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>1003</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>315</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>1061</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>339</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>1134</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>358</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="1"/>
+        <v>51</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>1212</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>381</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>1287</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>402</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" si="1"/>
+        <v>57</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>1365</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>426</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>1411</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>449</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>153</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>3000000</v>
+      </c>
+      <c r="B23">
+        <v>128108</v>
+      </c>
+      <c r="C23">
+        <v>26691</v>
+      </c>
+      <c r="D23">
+        <v>10424</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>6000000</v>
+      </c>
+      <c r="B24">
+        <v>209859</v>
+      </c>
+      <c r="C24">
+        <v>48949</v>
+      </c>
+      <c r="D24">
+        <v>17842</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>9000000</v>
+      </c>
+      <c r="B25">
+        <v>284329</v>
+      </c>
+      <c r="C25">
+        <v>71785</v>
+      </c>
+      <c r="D25">
+        <v>25883</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>12000000</v>
+      </c>
+      <c r="B26">
+        <v>356776</v>
+      </c>
+      <c r="C26">
+        <v>93098</v>
+      </c>
+      <c r="D26">
+        <v>33257</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>15000000</v>
+      </c>
+      <c r="B27">
+        <v>422941</v>
+      </c>
+      <c r="C27">
+        <v>116807</v>
+      </c>
+      <c r="D27">
+        <v>40349</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>18000000</v>
+      </c>
+      <c r="B28">
+        <v>500698</v>
+      </c>
+      <c r="C28">
+        <v>139044</v>
+      </c>
+      <c r="D28">
+        <v>48583</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>21000000</v>
+      </c>
+      <c r="B29">
+        <v>566406</v>
+      </c>
+      <c r="C29">
+        <v>160875</v>
+      </c>
+      <c r="D29">
+        <v>55987</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>24000000</v>
+      </c>
+      <c r="B30">
+        <v>642605</v>
+      </c>
+      <c r="C30">
+        <v>181225</v>
+      </c>
+      <c r="D30">
+        <v>62639</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>27000000</v>
+      </c>
+      <c r="B31">
+        <v>686193</v>
+      </c>
+      <c r="C31">
+        <v>204739</v>
+      </c>
+      <c r="D31">
+        <v>70711</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>30000000</v>
+      </c>
+      <c r="B32">
+        <v>741954</v>
+      </c>
+      <c r="C32">
+        <v>225674</v>
+      </c>
+      <c r="D32">
+        <v>77042</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>33000000</v>
+      </c>
+      <c r="B33">
+        <v>812220</v>
+      </c>
+      <c r="C33">
+        <v>248403</v>
+      </c>
+      <c r="D33">
+        <v>84666</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>36000000</v>
+      </c>
+      <c r="B34">
+        <v>891112</v>
+      </c>
+      <c r="C34">
+        <v>271096</v>
+      </c>
+      <c r="D34">
+        <v>93059</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>39000000</v>
+      </c>
+      <c r="B35">
+        <v>963793</v>
+      </c>
+      <c r="C35">
+        <v>294279</v>
+      </c>
+      <c r="D35">
+        <v>100442</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>42000000</v>
+      </c>
+      <c r="B36">
+        <v>1003222</v>
+      </c>
+      <c r="C36">
+        <v>315498</v>
+      </c>
+      <c r="D36">
+        <v>108916</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>45000000</v>
+      </c>
+      <c r="B37">
+        <v>1061405</v>
+      </c>
+      <c r="C37">
+        <v>338870</v>
+      </c>
+      <c r="D37">
+        <v>115025</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>48000000</v>
+      </c>
+      <c r="B38">
+        <v>1133993</v>
+      </c>
+      <c r="C38">
+        <v>358499</v>
+      </c>
+      <c r="D38">
+        <v>122539</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>51000000</v>
+      </c>
+      <c r="B39">
+        <v>1212411</v>
+      </c>
+      <c r="C39">
+        <v>381269</v>
+      </c>
+      <c r="D39">
+        <v>130936</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>54000000</v>
+      </c>
+      <c r="B40">
+        <v>1287491</v>
+      </c>
+      <c r="C40">
+        <v>401986</v>
+      </c>
+      <c r="D40">
+        <v>137429</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>57000000</v>
+      </c>
+      <c r="B41">
+        <v>1365236</v>
+      </c>
+      <c r="C41">
+        <v>425713</v>
+      </c>
+      <c r="D41">
+        <v>145062</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>60000000</v>
+      </c>
+      <c r="B42">
+        <v>1410681</v>
+      </c>
+      <c r="C42">
+        <v>448854</v>
+      </c>
+      <c r="D42">
+        <v>152902</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Code aufgeräumt und kommentiert, benchmarks für Umkreisabfrage implementiert und aufgenommen
</commit_message>
<xml_diff>
--- a/Laufzeit Benchmarks.xlsx
+++ b/Laufzeit Benchmarks.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7770" activeTab="4" xr2:uid="{CF6F9929-A31F-489D-9572-F5B799929CF5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7770" xr2:uid="{CF6F9929-A31F-489D-9572-F5B799929CF5}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
     <sheet name="Tabelle4" sheetId="4" r:id="rId4"/>
     <sheet name="Tabelle5" sheetId="5" r:id="rId5"/>
+    <sheet name="Tabelle7" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="51">
   <si>
     <t>Mit Daten kopieren</t>
   </si>
@@ -170,6 +171,18 @@
   <si>
     <t xml:space="preserve"> GPU mit kopieren</t>
   </si>
+  <si>
+    <t>Anfrage Radius</t>
+  </si>
+  <si>
+    <t>niedrigste gemessene Zeit bei 10 durchläufen</t>
+  </si>
+  <si>
+    <t>laser.00080.chkpt.density.mmpld</t>
+  </si>
+  <si>
+    <t>Anfrage Position zentriert</t>
+  </si>
 </sst>
 </file>
 
@@ -308,7 +321,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -375,6 +388,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -5824,7 +5838,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle5!$B$1</c:f>
+              <c:f>Tabelle5!$B$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5920,7 +5934,7 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>Tabelle5!$A$2:$A$21</c:f>
+              <c:f>Tabelle5!$A$16:$A$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -5989,7 +6003,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle5!$B$2:$B$21</c:f>
+              <c:f>Tabelle5!$B$16:$B$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -6068,7 +6082,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle5!$C$1</c:f>
+              <c:f>Tabelle5!$C$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6208,7 +6222,7 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>Tabelle5!$A$2:$A$21</c:f>
+              <c:f>Tabelle5!$A$16:$A$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -6277,7 +6291,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle5!$C$2:$C$21</c:f>
+              <c:f>Tabelle5!$C$16:$C$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -6356,7 +6370,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle5!$D$1</c:f>
+              <c:f>Tabelle5!$D$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6518,7 +6532,7 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>Tabelle5!$A$2:$A$21</c:f>
+              <c:f>Tabelle5!$A$16:$A$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -6587,7 +6601,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle5!$D$2:$D$21</c:f>
+              <c:f>Tabelle5!$D$16:$D$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -6999,6 +7013,844 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle7!$F$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v> GPU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Tabelle7!$E$19:$E$48</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>156</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>195</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>214</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>234</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>253</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>273</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>292</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>312</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>331</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>351</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>409</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>429</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>448</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>468</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>487</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>507</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>526</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>546</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>565</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>585</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle7!$F$19:$F$48</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>0.41299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.502</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.39400000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.47899999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.441</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.49</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.45200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.43</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.441</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.46500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.46600000000000003</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.44800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.47899999999999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.47599999999999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.47699999999999998</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.50700000000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.49099999999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.52400000000000002</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.55600000000000005</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.55500000000000005</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.54800000000000004</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.73599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.78500000000000003</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.85799999999999998</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.90600000000000003</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.93400000000000005</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.96699999999999997</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.0629999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6A14-4EF8-8B64-D9E603C259D5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle7!$G$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v> CPU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Tabelle7!$E$19:$E$48</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>156</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>195</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>214</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>234</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>253</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>273</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>292</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>312</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>331</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>351</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>409</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>429</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>448</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>468</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>487</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>507</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>526</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>546</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>565</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>585</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle7!$G$19:$G$48</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>1.6E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.5999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.5999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.153</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.26600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.441</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0609999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.244</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.385</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.5840000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.7709999999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.944</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.081</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.3370000000000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.4969999999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.798</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.0710000000000002</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.407</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.7290000000000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4.2320000000000002</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>6.25</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>8.9009999999999998</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>11.311</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>13.111000000000001</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>15.374000000000001</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>15.688000000000001</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>17.379000000000001</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>17.951000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6A14-4EF8-8B64-D9E603C259D5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="643236136"/>
+        <c:axId val="643236792"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="643236136"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Anfrage Radius</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="643236792"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="643236792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Laufzeit in ms</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="643236136"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -7199,6 +8051,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -9747,6 +10639,522 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -9951,6 +11359,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6272BB7C-5DA6-4559-8BD5-9F288248D974}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>114299</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>485774</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>80009</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F26432EC-5079-4E35-B37F-9E3AD4DD7ADE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10270,7 +11719,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DDBFD6F-1AC2-4396-A59E-40555DBC7422}">
   <dimension ref="A1:R22"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
@@ -11173,7 +12622,7 @@
   <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:E5"/>
+      <selection activeCell="A3" sqref="A3:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11433,8 +12882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{946918F2-691D-476E-85B8-BB2E0F70E0AC}">
   <dimension ref="A2:E113"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13237,10 +14686,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B451884F-F8BD-4F01-B10F-A7E0BAE46247}">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13248,661 +14697,1536 @@
     <col min="2" max="2" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="50" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="51"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="45">
+        <v>0</v>
+      </c>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="46"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="46"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="45" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="46"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="45" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="46"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="46"/>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="48"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>25</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B15" t="s">
         <v>44</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C15" t="s">
         <v>46</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D15" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <f>A23/1000000</f>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f>A37/1000000</f>
         <v>3</v>
       </c>
-      <c r="B2">
-        <f t="shared" ref="B2:D21" si="0">ROUND(B23/1000, 0)</f>
+      <c r="B16">
+        <f t="shared" ref="B16:D35" si="0">ROUND(B37/1000, 0)</f>
         <v>128</v>
       </c>
-      <c r="C2">
+      <c r="C16">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="D2">
+      <c r="D16">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <f t="shared" ref="A3:A21" si="1">A24/1000000</f>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" ref="A17:A35" si="1">A38/1000000</f>
         <v>6</v>
       </c>
-      <c r="B3">
+      <c r="B17">
         <f t="shared" si="0"/>
         <v>210</v>
       </c>
-      <c r="C3">
+      <c r="C17">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="D3">
+      <c r="D17">
         <f t="shared" si="0"/>
         <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="B4">
-        <f t="shared" si="0"/>
-        <v>284</v>
-      </c>
-      <c r="C4">
-        <f t="shared" si="0"/>
-        <v>72</v>
-      </c>
-      <c r="D4">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="B5">
-        <f t="shared" si="0"/>
-        <v>357</v>
-      </c>
-      <c r="C5">
-        <f t="shared" si="0"/>
-        <v>93</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="B6">
-        <f t="shared" si="0"/>
-        <v>423</v>
-      </c>
-      <c r="C6">
-        <f t="shared" si="0"/>
-        <v>117</v>
-      </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="B7">
-        <f t="shared" si="0"/>
-        <v>501</v>
-      </c>
-      <c r="C7">
-        <f t="shared" si="0"/>
-        <v>139</v>
-      </c>
-      <c r="D7">
-        <f t="shared" si="0"/>
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <f t="shared" si="1"/>
-        <v>21</v>
-      </c>
-      <c r="B8">
-        <f t="shared" si="0"/>
-        <v>566</v>
-      </c>
-      <c r="C8">
-        <f t="shared" si="0"/>
-        <v>161</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="0"/>
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <f t="shared" si="1"/>
-        <v>24</v>
-      </c>
-      <c r="B9">
-        <f t="shared" si="0"/>
-        <v>643</v>
-      </c>
-      <c r="C9">
-        <f t="shared" si="0"/>
-        <v>181</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <f t="shared" si="1"/>
-        <v>27</v>
-      </c>
-      <c r="B10">
-        <f t="shared" si="0"/>
-        <v>686</v>
-      </c>
-      <c r="C10">
-        <f t="shared" si="0"/>
-        <v>205</v>
-      </c>
-      <c r="D10">
-        <f t="shared" si="0"/>
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <f t="shared" si="1"/>
-        <v>30</v>
-      </c>
-      <c r="B11">
-        <f t="shared" si="0"/>
-        <v>742</v>
-      </c>
-      <c r="C11">
-        <f t="shared" si="0"/>
-        <v>226</v>
-      </c>
-      <c r="D11">
-        <f t="shared" si="0"/>
-        <v>77</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <f t="shared" si="1"/>
-        <v>33</v>
-      </c>
-      <c r="B12">
-        <f t="shared" si="0"/>
-        <v>812</v>
-      </c>
-      <c r="C12">
-        <f t="shared" si="0"/>
-        <v>248</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="0"/>
-        <v>85</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <f t="shared" si="1"/>
-        <v>36</v>
-      </c>
-      <c r="B13">
-        <f t="shared" si="0"/>
-        <v>891</v>
-      </c>
-      <c r="C13">
-        <f t="shared" si="0"/>
-        <v>271</v>
-      </c>
-      <c r="D13">
-        <f t="shared" si="0"/>
-        <v>93</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <f t="shared" si="1"/>
-        <v>39</v>
-      </c>
-      <c r="B14">
-        <f t="shared" si="0"/>
-        <v>964</v>
-      </c>
-      <c r="C14">
-        <f t="shared" si="0"/>
-        <v>294</v>
-      </c>
-      <c r="D14">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <f t="shared" si="1"/>
-        <v>42</v>
-      </c>
-      <c r="B15">
-        <f t="shared" si="0"/>
-        <v>1003</v>
-      </c>
-      <c r="C15">
-        <f t="shared" si="0"/>
-        <v>315</v>
-      </c>
-      <c r="D15">
-        <f t="shared" si="0"/>
-        <v>109</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <f t="shared" si="1"/>
-        <v>45</v>
-      </c>
-      <c r="B16">
-        <f t="shared" si="0"/>
-        <v>1061</v>
-      </c>
-      <c r="C16">
-        <f t="shared" si="0"/>
-        <v>339</v>
-      </c>
-      <c r="D16">
-        <f t="shared" si="0"/>
-        <v>115</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <f t="shared" si="1"/>
-        <v>48</v>
-      </c>
-      <c r="B17">
-        <f t="shared" si="0"/>
-        <v>1134</v>
-      </c>
-      <c r="C17">
-        <f t="shared" si="0"/>
-        <v>358</v>
-      </c>
-      <c r="D17">
-        <f t="shared" si="0"/>
-        <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="1"/>
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="B18">
         <f t="shared" si="0"/>
-        <v>1212</v>
+        <v>284</v>
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>381</v>
+        <v>72</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>131</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="1"/>
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="B19">
         <f t="shared" si="0"/>
-        <v>1287</v>
+        <v>357</v>
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>402</v>
+        <v>93</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>137</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="1"/>
-        <v>57</v>
+        <v>15</v>
       </c>
       <c r="B20">
         <f t="shared" si="0"/>
-        <v>1365</v>
+        <v>423</v>
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>426</v>
+        <v>117</v>
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
-        <v>145</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="1"/>
-        <v>60</v>
+        <v>18</v>
       </c>
       <c r="B21">
         <f t="shared" si="0"/>
-        <v>1411</v>
+        <v>501</v>
       </c>
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>449</v>
+        <v>139</v>
       </c>
       <c r="D21">
         <f t="shared" si="0"/>
-        <v>153</v>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>566</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>161</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>3000000</v>
+        <f t="shared" si="1"/>
+        <v>24</v>
       </c>
       <c r="B23">
-        <v>128108</v>
+        <f t="shared" si="0"/>
+        <v>643</v>
       </c>
       <c r="C23">
-        <v>26691</v>
+        <f t="shared" si="0"/>
+        <v>181</v>
       </c>
       <c r="D23">
-        <v>10424</v>
+        <f t="shared" si="0"/>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>6000000</v>
+        <f t="shared" si="1"/>
+        <v>27</v>
       </c>
       <c r="B24">
-        <v>209859</v>
+        <f t="shared" si="0"/>
+        <v>686</v>
       </c>
       <c r="C24">
-        <v>48949</v>
+        <f t="shared" si="0"/>
+        <v>205</v>
       </c>
       <c r="D24">
-        <v>17842</v>
+        <f t="shared" si="0"/>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>9000000</v>
+        <f t="shared" si="1"/>
+        <v>30</v>
       </c>
       <c r="B25">
-        <v>284329</v>
+        <f t="shared" si="0"/>
+        <v>742</v>
       </c>
       <c r="C25">
-        <v>71785</v>
+        <f t="shared" si="0"/>
+        <v>226</v>
       </c>
       <c r="D25">
-        <v>25883</v>
+        <f t="shared" si="0"/>
+        <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>12000000</v>
+        <f t="shared" si="1"/>
+        <v>33</v>
       </c>
       <c r="B26">
-        <v>356776</v>
+        <f t="shared" si="0"/>
+        <v>812</v>
       </c>
       <c r="C26">
-        <v>93098</v>
+        <f t="shared" si="0"/>
+        <v>248</v>
       </c>
       <c r="D26">
-        <v>33257</v>
+        <f t="shared" si="0"/>
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>15000000</v>
+        <f t="shared" si="1"/>
+        <v>36</v>
       </c>
       <c r="B27">
-        <v>422941</v>
+        <f t="shared" si="0"/>
+        <v>891</v>
       </c>
       <c r="C27">
-        <v>116807</v>
+        <f t="shared" si="0"/>
+        <v>271</v>
       </c>
       <c r="D27">
-        <v>40349</v>
+        <f t="shared" si="0"/>
+        <v>93</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>18000000</v>
+        <f t="shared" si="1"/>
+        <v>39</v>
       </c>
       <c r="B28">
-        <v>500698</v>
+        <f t="shared" si="0"/>
+        <v>964</v>
       </c>
       <c r="C28">
-        <v>139044</v>
+        <f t="shared" si="0"/>
+        <v>294</v>
       </c>
       <c r="D28">
-        <v>48583</v>
+        <f t="shared" si="0"/>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>21000000</v>
+        <f t="shared" si="1"/>
+        <v>42</v>
       </c>
       <c r="B29">
-        <v>566406</v>
+        <f t="shared" si="0"/>
+        <v>1003</v>
       </c>
       <c r="C29">
-        <v>160875</v>
+        <f t="shared" si="0"/>
+        <v>315</v>
       </c>
       <c r="D29">
-        <v>55987</v>
+        <f t="shared" si="0"/>
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>24000000</v>
+        <f t="shared" si="1"/>
+        <v>45</v>
       </c>
       <c r="B30">
-        <v>642605</v>
+        <f t="shared" si="0"/>
+        <v>1061</v>
       </c>
       <c r="C30">
-        <v>181225</v>
+        <f t="shared" si="0"/>
+        <v>339</v>
       </c>
       <c r="D30">
-        <v>62639</v>
+        <f t="shared" si="0"/>
+        <v>115</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>27000000</v>
+        <f t="shared" si="1"/>
+        <v>48</v>
       </c>
       <c r="B31">
-        <v>686193</v>
+        <f t="shared" si="0"/>
+        <v>1134</v>
       </c>
       <c r="C31">
-        <v>204739</v>
+        <f t="shared" si="0"/>
+        <v>358</v>
       </c>
       <c r="D31">
-        <v>70711</v>
+        <f t="shared" si="0"/>
+        <v>123</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>30000000</v>
+        <f t="shared" si="1"/>
+        <v>51</v>
       </c>
       <c r="B32">
-        <v>741954</v>
+        <f t="shared" si="0"/>
+        <v>1212</v>
       </c>
       <c r="C32">
-        <v>225674</v>
+        <f t="shared" si="0"/>
+        <v>381</v>
       </c>
       <c r="D32">
-        <v>77042</v>
+        <f t="shared" si="0"/>
+        <v>131</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>33000000</v>
+        <f t="shared" si="1"/>
+        <v>54</v>
       </c>
       <c r="B33">
-        <v>812220</v>
+        <f t="shared" si="0"/>
+        <v>1287</v>
       </c>
       <c r="C33">
-        <v>248403</v>
+        <f t="shared" si="0"/>
+        <v>402</v>
       </c>
       <c r="D33">
-        <v>84666</v>
+        <f t="shared" si="0"/>
+        <v>137</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>36000000</v>
+        <f t="shared" si="1"/>
+        <v>57</v>
       </c>
       <c r="B34">
-        <v>891112</v>
+        <f t="shared" si="0"/>
+        <v>1365</v>
       </c>
       <c r="C34">
-        <v>271096</v>
+        <f t="shared" si="0"/>
+        <v>426</v>
       </c>
       <c r="D34">
-        <v>93059</v>
+        <f t="shared" si="0"/>
+        <v>145</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>39000000</v>
+        <f t="shared" si="1"/>
+        <v>60</v>
       </c>
       <c r="B35">
-        <v>963793</v>
+        <f t="shared" si="0"/>
+        <v>1411</v>
       </c>
       <c r="C35">
-        <v>294279</v>
+        <f t="shared" si="0"/>
+        <v>449</v>
       </c>
       <c r="D35">
-        <v>100442</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>42000000</v>
-      </c>
-      <c r="B36">
-        <v>1003222</v>
-      </c>
-      <c r="C36">
-        <v>315498</v>
-      </c>
-      <c r="D36">
-        <v>108916</v>
+        <f t="shared" si="0"/>
+        <v>153</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>45000000</v>
+        <v>3000000</v>
       </c>
       <c r="B37">
-        <v>1061405</v>
+        <v>128108</v>
       </c>
       <c r="C37">
-        <v>338870</v>
+        <v>26691</v>
       </c>
       <c r="D37">
-        <v>115025</v>
+        <v>10424</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>48000000</v>
+        <v>6000000</v>
       </c>
       <c r="B38">
-        <v>1133993</v>
+        <v>209859</v>
       </c>
       <c r="C38">
-        <v>358499</v>
+        <v>48949</v>
       </c>
       <c r="D38">
-        <v>122539</v>
+        <v>17842</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>51000000</v>
+        <v>9000000</v>
       </c>
       <c r="B39">
-        <v>1212411</v>
+        <v>284329</v>
       </c>
       <c r="C39">
-        <v>381269</v>
+        <v>71785</v>
       </c>
       <c r="D39">
-        <v>130936</v>
+        <v>25883</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>54000000</v>
+        <v>12000000</v>
       </c>
       <c r="B40">
-        <v>1287491</v>
+        <v>356776</v>
       </c>
       <c r="C40">
-        <v>401986</v>
+        <v>93098</v>
       </c>
       <c r="D40">
-        <v>137429</v>
+        <v>33257</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>57000000</v>
+        <v>15000000</v>
       </c>
       <c r="B41">
-        <v>1365236</v>
+        <v>422941</v>
       </c>
       <c r="C41">
-        <v>425713</v>
+        <v>116807</v>
       </c>
       <c r="D41">
-        <v>145062</v>
+        <v>40349</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
+        <v>18000000</v>
+      </c>
+      <c r="B42">
+        <v>500698</v>
+      </c>
+      <c r="C42">
+        <v>139044</v>
+      </c>
+      <c r="D42">
+        <v>48583</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>21000000</v>
+      </c>
+      <c r="B43">
+        <v>566406</v>
+      </c>
+      <c r="C43">
+        <v>160875</v>
+      </c>
+      <c r="D43">
+        <v>55987</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>24000000</v>
+      </c>
+      <c r="B44">
+        <v>642605</v>
+      </c>
+      <c r="C44">
+        <v>181225</v>
+      </c>
+      <c r="D44">
+        <v>62639</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>27000000</v>
+      </c>
+      <c r="B45">
+        <v>686193</v>
+      </c>
+      <c r="C45">
+        <v>204739</v>
+      </c>
+      <c r="D45">
+        <v>70711</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>30000000</v>
+      </c>
+      <c r="B46">
+        <v>741954</v>
+      </c>
+      <c r="C46">
+        <v>225674</v>
+      </c>
+      <c r="D46">
+        <v>77042</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>33000000</v>
+      </c>
+      <c r="B47">
+        <v>812220</v>
+      </c>
+      <c r="C47">
+        <v>248403</v>
+      </c>
+      <c r="D47">
+        <v>84666</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>36000000</v>
+      </c>
+      <c r="B48">
+        <v>891112</v>
+      </c>
+      <c r="C48">
+        <v>271096</v>
+      </c>
+      <c r="D48">
+        <v>93059</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>39000000</v>
+      </c>
+      <c r="B49">
+        <v>963793</v>
+      </c>
+      <c r="C49">
+        <v>294279</v>
+      </c>
+      <c r="D49">
+        <v>100442</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>42000000</v>
+      </c>
+      <c r="B50">
+        <v>1003222</v>
+      </c>
+      <c r="C50">
+        <v>315498</v>
+      </c>
+      <c r="D50">
+        <v>108916</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>45000000</v>
+      </c>
+      <c r="B51">
+        <v>1061405</v>
+      </c>
+      <c r="C51">
+        <v>338870</v>
+      </c>
+      <c r="D51">
+        <v>115025</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>48000000</v>
+      </c>
+      <c r="B52">
+        <v>1133993</v>
+      </c>
+      <c r="C52">
+        <v>358499</v>
+      </c>
+      <c r="D52">
+        <v>122539</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>51000000</v>
+      </c>
+      <c r="B53">
+        <v>1212411</v>
+      </c>
+      <c r="C53">
+        <v>381269</v>
+      </c>
+      <c r="D53">
+        <v>130936</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>54000000</v>
+      </c>
+      <c r="B54">
+        <v>1287491</v>
+      </c>
+      <c r="C54">
+        <v>401986</v>
+      </c>
+      <c r="D54">
+        <v>137429</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>57000000</v>
+      </c>
+      <c r="B55">
+        <v>1365236</v>
+      </c>
+      <c r="C55">
+        <v>425713</v>
+      </c>
+      <c r="D55">
+        <v>145062</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56">
         <v>60000000</v>
       </c>
+      <c r="B56">
+        <v>1410681</v>
+      </c>
+      <c r="C56">
+        <v>448854</v>
+      </c>
+      <c r="D56">
+        <v>152902</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F077C225-171D-430F-9D38-9B5D3C2625F3}">
+  <dimension ref="A1:G48"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18:G48"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="51"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="45">
+        <v>200</v>
+      </c>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="46"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="45">
+        <v>562500</v>
+      </c>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="46"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="45" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="46"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="45" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="46"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="46"/>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="48"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="52" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" t="s">
+        <v>45</v>
+      </c>
+      <c r="G18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <v>413</v>
+      </c>
+      <c r="C19">
+        <v>16</v>
+      </c>
+      <c r="E19">
+        <v>19</v>
+      </c>
+      <c r="F19">
+        <f>B19/1000</f>
+        <v>0.41299999999999998</v>
+      </c>
+      <c r="G19">
+        <f>C19/1000</f>
+        <v>1.6E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>39</v>
+      </c>
+      <c r="B20">
+        <v>502</v>
+      </c>
+      <c r="C20">
+        <v>36</v>
+      </c>
+      <c r="E20">
+        <v>39</v>
+      </c>
+      <c r="F20">
+        <f>B20/1000</f>
+        <v>0.502</v>
+      </c>
+      <c r="G20">
+        <f>C20/1000</f>
+        <v>3.5999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>58</v>
+      </c>
+      <c r="B21">
+        <v>394</v>
+      </c>
+      <c r="C21">
+        <v>76</v>
+      </c>
+      <c r="E21">
+        <v>58</v>
+      </c>
+      <c r="F21">
+        <f>B21/1000</f>
+        <v>0.39400000000000002</v>
+      </c>
+      <c r="G21">
+        <f>C21/1000</f>
+        <v>7.5999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>78</v>
+      </c>
+      <c r="B22">
+        <v>400</v>
+      </c>
+      <c r="C22">
+        <v>153</v>
+      </c>
+      <c r="E22">
+        <v>78</v>
+      </c>
+      <c r="F22">
+        <f>B22/1000</f>
+        <v>0.4</v>
+      </c>
+      <c r="G22">
+        <f>C22/1000</f>
+        <v>0.153</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>97</v>
+      </c>
+      <c r="B23">
+        <v>479</v>
+      </c>
+      <c r="C23">
+        <v>266</v>
+      </c>
+      <c r="E23">
+        <v>97</v>
+      </c>
+      <c r="F23">
+        <f>B23/1000</f>
+        <v>0.47899999999999998</v>
+      </c>
+      <c r="G23">
+        <f>C23/1000</f>
+        <v>0.26600000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>117</v>
+      </c>
+      <c r="B24">
+        <v>441</v>
+      </c>
+      <c r="C24">
+        <v>441</v>
+      </c>
+      <c r="E24">
+        <v>117</v>
+      </c>
+      <c r="F24">
+        <f>B24/1000</f>
+        <v>0.441</v>
+      </c>
+      <c r="G24">
+        <f>C24/1000</f>
+        <v>0.441</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>136</v>
+      </c>
+      <c r="B25">
+        <v>490</v>
+      </c>
+      <c r="C25">
+        <v>700</v>
+      </c>
+      <c r="E25">
+        <v>136</v>
+      </c>
+      <c r="F25">
+        <f>B25/1000</f>
+        <v>0.49</v>
+      </c>
+      <c r="G25">
+        <f>C25/1000</f>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>156</v>
+      </c>
+      <c r="B26">
+        <v>452</v>
+      </c>
+      <c r="C26">
+        <v>940</v>
+      </c>
+      <c r="E26">
+        <v>156</v>
+      </c>
+      <c r="F26">
+        <f>B26/1000</f>
+        <v>0.45200000000000001</v>
+      </c>
+      <c r="G26">
+        <f>C26/1000</f>
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>175</v>
+      </c>
+      <c r="B27">
+        <v>430</v>
+      </c>
+      <c r="C27">
+        <v>1061</v>
+      </c>
+      <c r="E27">
+        <v>175</v>
+      </c>
+      <c r="F27">
+        <f>B27/1000</f>
+        <v>0.43</v>
+      </c>
+      <c r="G27">
+        <f>C27/1000</f>
+        <v>1.0609999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>195</v>
+      </c>
+      <c r="B28">
+        <v>441</v>
+      </c>
+      <c r="C28">
+        <v>1244</v>
+      </c>
+      <c r="E28">
+        <v>195</v>
+      </c>
+      <c r="F28">
+        <f>B28/1000</f>
+        <v>0.441</v>
+      </c>
+      <c r="G28">
+        <f>C28/1000</f>
+        <v>1.244</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>214</v>
+      </c>
+      <c r="B29">
+        <v>465</v>
+      </c>
+      <c r="C29">
+        <v>1385</v>
+      </c>
+      <c r="E29">
+        <v>214</v>
+      </c>
+      <c r="F29">
+        <f>B29/1000</f>
+        <v>0.46500000000000002</v>
+      </c>
+      <c r="G29">
+        <f>C29/1000</f>
+        <v>1.385</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>234</v>
+      </c>
+      <c r="B30">
+        <v>466</v>
+      </c>
+      <c r="C30">
+        <v>1584</v>
+      </c>
+      <c r="E30">
+        <v>234</v>
+      </c>
+      <c r="F30">
+        <f>B30/1000</f>
+        <v>0.46600000000000003</v>
+      </c>
+      <c r="G30">
+        <f>C30/1000</f>
+        <v>1.5840000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>253</v>
+      </c>
+      <c r="B31">
+        <v>448</v>
+      </c>
+      <c r="C31">
+        <v>1771</v>
+      </c>
+      <c r="E31">
+        <v>253</v>
+      </c>
+      <c r="F31">
+        <f>B31/1000</f>
+        <v>0.44800000000000001</v>
+      </c>
+      <c r="G31">
+        <f>C31/1000</f>
+        <v>1.7709999999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>273</v>
+      </c>
+      <c r="B32">
+        <v>479</v>
+      </c>
+      <c r="C32">
+        <v>1944</v>
+      </c>
+      <c r="E32">
+        <v>273</v>
+      </c>
+      <c r="F32">
+        <f>B32/1000</f>
+        <v>0.47899999999999998</v>
+      </c>
+      <c r="G32">
+        <f>C32/1000</f>
+        <v>1.944</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>292</v>
+      </c>
+      <c r="B33">
+        <v>476</v>
+      </c>
+      <c r="C33">
+        <v>2081</v>
+      </c>
+      <c r="E33">
+        <v>292</v>
+      </c>
+      <c r="F33">
+        <f>B33/1000</f>
+        <v>0.47599999999999998</v>
+      </c>
+      <c r="G33">
+        <f>C33/1000</f>
+        <v>2.081</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>312</v>
+      </c>
+      <c r="B34">
+        <v>477</v>
+      </c>
+      <c r="C34">
+        <v>2337</v>
+      </c>
+      <c r="E34">
+        <v>312</v>
+      </c>
+      <c r="F34">
+        <f>B34/1000</f>
+        <v>0.47699999999999998</v>
+      </c>
+      <c r="G34">
+        <f>C34/1000</f>
+        <v>2.3370000000000002</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>331</v>
+      </c>
+      <c r="B35">
+        <v>507</v>
+      </c>
+      <c r="C35">
+        <v>2497</v>
+      </c>
+      <c r="E35">
+        <v>331</v>
+      </c>
+      <c r="F35">
+        <f>B35/1000</f>
+        <v>0.50700000000000001</v>
+      </c>
+      <c r="G35">
+        <f>C35/1000</f>
+        <v>2.4969999999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>351</v>
+      </c>
+      <c r="B36">
+        <v>491</v>
+      </c>
+      <c r="C36">
+        <v>2798</v>
+      </c>
+      <c r="E36">
+        <v>351</v>
+      </c>
+      <c r="F36">
+        <f>B36/1000</f>
+        <v>0.49099999999999999</v>
+      </c>
+      <c r="G36">
+        <f>C36/1000</f>
+        <v>2.798</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>370</v>
+      </c>
+      <c r="B37">
+        <v>524</v>
+      </c>
+      <c r="C37">
+        <v>3071</v>
+      </c>
+      <c r="E37">
+        <v>370</v>
+      </c>
+      <c r="F37">
+        <f>B37/1000</f>
+        <v>0.52400000000000002</v>
+      </c>
+      <c r="G37">
+        <f>C37/1000</f>
+        <v>3.0710000000000002</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>390</v>
+      </c>
+      <c r="B38">
+        <v>556</v>
+      </c>
+      <c r="C38">
+        <v>3407</v>
+      </c>
+      <c r="E38">
+        <v>390</v>
+      </c>
+      <c r="F38">
+        <f>B38/1000</f>
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="G38">
+        <f>C38/1000</f>
+        <v>3.407</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>409</v>
+      </c>
+      <c r="B39">
+        <v>555</v>
+      </c>
+      <c r="C39">
+        <v>3729</v>
+      </c>
+      <c r="E39">
+        <v>409</v>
+      </c>
+      <c r="F39">
+        <f>B39/1000</f>
+        <v>0.55500000000000005</v>
+      </c>
+      <c r="G39">
+        <f>C39/1000</f>
+        <v>3.7290000000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>429</v>
+      </c>
+      <c r="B40">
+        <v>548</v>
+      </c>
+      <c r="C40">
+        <v>4232</v>
+      </c>
+      <c r="E40">
+        <v>429</v>
+      </c>
+      <c r="F40">
+        <f>B40/1000</f>
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="G40">
+        <f>C40/1000</f>
+        <v>4.2320000000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>448</v>
+      </c>
+      <c r="B41">
+        <v>736</v>
+      </c>
+      <c r="C41">
+        <v>6250</v>
+      </c>
+      <c r="E41">
+        <v>448</v>
+      </c>
+      <c r="F41">
+        <f>B41/1000</f>
+        <v>0.73599999999999999</v>
+      </c>
+      <c r="G41">
+        <f>C41/1000</f>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>468</v>
+      </c>
       <c r="B42">
-        <v>1410681</v>
+        <v>785</v>
       </c>
       <c r="C42">
-        <v>448854</v>
-      </c>
-      <c r="D42">
-        <v>152902</v>
+        <v>8901</v>
+      </c>
+      <c r="E42">
+        <v>468</v>
+      </c>
+      <c r="F42">
+        <f>B42/1000</f>
+        <v>0.78500000000000003</v>
+      </c>
+      <c r="G42">
+        <f>C42/1000</f>
+        <v>8.9009999999999998</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>487</v>
+      </c>
+      <c r="B43">
+        <v>858</v>
+      </c>
+      <c r="C43">
+        <v>11311</v>
+      </c>
+      <c r="E43">
+        <v>487</v>
+      </c>
+      <c r="F43">
+        <f>B43/1000</f>
+        <v>0.85799999999999998</v>
+      </c>
+      <c r="G43">
+        <f>C43/1000</f>
+        <v>11.311</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>507</v>
+      </c>
+      <c r="B44">
+        <v>906</v>
+      </c>
+      <c r="C44">
+        <v>13111</v>
+      </c>
+      <c r="E44">
+        <v>507</v>
+      </c>
+      <c r="F44">
+        <f>B44/1000</f>
+        <v>0.90600000000000003</v>
+      </c>
+      <c r="G44">
+        <f>C44/1000</f>
+        <v>13.111000000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>526</v>
+      </c>
+      <c r="B45">
+        <v>934</v>
+      </c>
+      <c r="C45">
+        <v>15374</v>
+      </c>
+      <c r="E45">
+        <v>526</v>
+      </c>
+      <c r="F45">
+        <f>B45/1000</f>
+        <v>0.93400000000000005</v>
+      </c>
+      <c r="G45">
+        <f>C45/1000</f>
+        <v>15.374000000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>546</v>
+      </c>
+      <c r="B46">
+        <v>967</v>
+      </c>
+      <c r="C46">
+        <v>15688</v>
+      </c>
+      <c r="E46">
+        <v>546</v>
+      </c>
+      <c r="F46">
+        <f>B46/1000</f>
+        <v>0.96699999999999997</v>
+      </c>
+      <c r="G46">
+        <f>C46/1000</f>
+        <v>15.688000000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>565</v>
+      </c>
+      <c r="B47">
+        <v>980</v>
+      </c>
+      <c r="C47">
+        <v>17379</v>
+      </c>
+      <c r="E47">
+        <v>565</v>
+      </c>
+      <c r="F47">
+        <f>B47/1000</f>
+        <v>0.98</v>
+      </c>
+      <c r="G47">
+        <f>C47/1000</f>
+        <v>17.379000000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>585</v>
+      </c>
+      <c r="B48">
+        <v>1063</v>
+      </c>
+      <c r="C48">
+        <v>17951</v>
+      </c>
+      <c r="E48">
+        <v>585</v>
+      </c>
+      <c r="F48">
+        <f>B48/1000</f>
+        <v>1.0629999999999999</v>
+      </c>
+      <c r="G48">
+        <f>C48/1000</f>
+        <v>17.951000000000001</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>